<commit_message>
on 31-10-2017 on localhost
</commit_message>
<xml_diff>
--- a/public/Download Excel Questions File.xlsx
+++ b/public/Download Excel Questions File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">option D</t>
   </si>
   <si>
+    <t xml:space="preserve">option E</t>
+  </si>
+  <si>
     <t xml:space="preserve">right answer</t>
   </si>
   <si>
@@ -46,9 +49,6 @@
     <t xml:space="preserve">max</t>
   </si>
   <si>
-    <t xml:space="preserve">section_type</t>
-  </si>
-  <si>
     <t xml:space="preserve">question_type</t>
   </si>
   <si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">negative_mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common_data</t>
   </si>
 </sst>
 </file>
@@ -73,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,22 +158,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8520408163265"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,6 +215,9 @@
       </c>
       <c r="M1" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>